<commit_message>
login + import khối kiến thức
</commit_message>
<xml_diff>
--- a/public/TemplateImport/template_import_subject.xlsx
+++ b/public/TemplateImport/template_import_subject.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\learning-app\public\TemplateImport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\learning-app\public\TemplateImport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F902F6AD-A270-4168-9A88-AB763FED7C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553D76BA-B5E9-4230-9822-1E313D0F7E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{087D9E47-7B34-47D3-8A7D-01AE6CA50FA8}"/>
+    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="11947" xr2:uid="{087D9E47-7B34-47D3-8A7D-01AE6CA50FA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>DEF</t>
   </si>
@@ -47,47 +47,38 @@
     <t>Tên môn học</t>
   </si>
   <si>
-    <t xml:space="preserve">Bắt buộc </t>
-  </si>
-  <si>
     <t>Mã môn học trước</t>
   </si>
   <si>
     <t>Mã môn học tương đương</t>
   </si>
   <si>
-    <t>Mã thành phần khung</t>
-  </si>
-  <si>
     <t>Số tín chỉ</t>
   </si>
   <si>
-    <t xml:space="preserve"> SubjectId</t>
-  </si>
-  <si>
-    <t>SubjectName</t>
-  </si>
-  <si>
-    <t>CreadHour</t>
-  </si>
-  <si>
-    <t>IsCompulsory</t>
-  </si>
-  <si>
-    <t>SubjectBeforeId</t>
-  </si>
-  <si>
-    <t>SubjectEqualId</t>
-  </si>
-  <si>
-    <t>FrameComponentId</t>
+    <t>IMPORT MÔN HỌC</t>
+  </si>
+  <si>
+    <t>subjectId</t>
+  </si>
+  <si>
+    <t>subjectName</t>
+  </si>
+  <si>
+    <t>creditHour</t>
+  </si>
+  <si>
+    <t>subjectBefore</t>
+  </si>
+  <si>
+    <t>subjectEqual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,19 +88,39 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,37 +140,48 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -492,93 +514,321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01DBA273-47A2-4126-A988-E125690B883F}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:T199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="D2" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47" style="1" customWidth="1"/>
-    <col min="2" max="2" width="46.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="19.1796875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="30.26953125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="17" style="6" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="24.6328125" style="6" customWidth="1"/>
+    <col min="6" max="20" width="9" style="7"/>
+    <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="36.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+    </row>
+    <row r="2" spans="1:20" ht="20.05" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="1:20" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" ht="20.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>123</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>123</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>3</v>
-      </c>
-      <c r="D3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
+    <row r="5" spans="1:20" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:20" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:20" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:20" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:20" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:20" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:20" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:20" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:20" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:20" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:20" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:20" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="20.05" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3" xr:uid="{0950E803-498F-427A-BF97-44D6A4894B42}">
-      <formula1>"True,False"</formula1>
-    </dataValidation>
-  </dataValidations>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>